<commit_message>
search bar and update suggestion
</commit_message>
<xml_diff>
--- a/api/courses.xlsx
+++ b/api/courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMHai\Desktop\uniquiry\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD72BB62-F8A0-4720-9B26-4E23E1F1F267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531A9A32-C443-4CD0-BE5F-C84DDEBB8048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1485" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="177">
   <si>
     <t>code</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>boundary</t>
   </si>
 </sst>
 </file>
@@ -916,15 +919,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -953,16 +956,19 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -990,17 +996,20 @@
       <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2">
-        <v>5000</v>
+      <c r="J2" s="1">
+        <v>85</v>
       </c>
       <c r="K2" s="2">
         <v>5000</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2">
+        <v>5000</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1028,17 +1037,20 @@
       <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
+        <v>85</v>
+      </c>
+      <c r="K3" s="2">
         <v>5243</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>5000</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1066,17 +1078,20 @@
       <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
+        <v>85</v>
+      </c>
+      <c r="K4" s="2">
         <v>4500</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>4228</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -1104,17 +1119,20 @@
       <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
+        <v>85</v>
+      </c>
+      <c r="K5" s="2">
         <v>5000</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>4228</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1142,17 +1160,20 @@
       <c r="I6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
+        <v>83.75</v>
+      </c>
+      <c r="K6" s="2">
         <v>5000</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>4000</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -1180,17 +1201,20 @@
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="1">
+        <v>75</v>
+      </c>
+      <c r="K7" s="4">
         <v>3500</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>3500</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1218,17 +1242,20 @@
       <c r="I8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
+        <v>76.25</v>
+      </c>
+      <c r="K8" s="2">
         <v>4000</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>3950</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1256,17 +1283,20 @@
       <c r="I9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
+        <v>67.5</v>
+      </c>
+      <c r="K9" s="2">
         <v>3590</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>3600</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -1294,17 +1324,20 @@
       <c r="I10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
+        <v>73.25</v>
+      </c>
+      <c r="K10" s="2">
         <v>4200</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>4000</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>60</v>
       </c>
@@ -1332,17 +1365,20 @@
       <c r="I11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
+        <v>73.25</v>
+      </c>
+      <c r="K11" s="2">
         <v>4000</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>3750</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>64</v>
       </c>
@@ -1370,17 +1406,20 @@
       <c r="I12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
+        <v>72</v>
+      </c>
+      <c r="K12" s="2">
         <v>3500</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>3400</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>69</v>
       </c>
@@ -1408,17 +1447,20 @@
       <c r="I13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
+        <v>72</v>
+      </c>
+      <c r="K13" s="2">
         <v>4380</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>4000</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -1446,17 +1488,20 @@
       <c r="I14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
+        <v>72</v>
+      </c>
+      <c r="K14" s="2">
         <v>3900</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>4000</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -1484,17 +1529,20 @@
       <c r="I15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
+        <v>73.25</v>
+      </c>
+      <c r="K15" s="2">
         <v>3800</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>3700</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
@@ -1522,17 +1570,20 @@
       <c r="I16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K16" s="2">
         <v>3528</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>3500</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>84</v>
       </c>
@@ -1560,17 +1611,20 @@
       <c r="I17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K17" s="2">
         <v>4125</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -1598,17 +1652,20 @@
       <c r="I18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K18" s="2">
         <v>3528</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>91</v>
       </c>
@@ -1636,17 +1693,20 @@
       <c r="I19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K19" s="2">
         <v>3250</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>3325</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>95</v>
       </c>
@@ -1674,17 +1734,20 @@
       <c r="I20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
+        <v>85</v>
+      </c>
+      <c r="K20" s="2">
         <v>3528</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>3500</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>99</v>
       </c>
@@ -1712,17 +1775,20 @@
       <c r="I21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K21" s="2">
         <v>3528</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>3500</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>102</v>
       </c>
@@ -1750,17 +1816,20 @@
       <c r="I22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K22" s="2">
         <v>3528</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>3500</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="M22" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>106</v>
       </c>
@@ -1788,17 +1857,20 @@
       <c r="I23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="1">
+        <v>85</v>
+      </c>
+      <c r="K23" s="2">
         <v>3528</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>3500</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>109</v>
       </c>
@@ -1826,17 +1898,20 @@
       <c r="I24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K24" s="2">
         <v>3528</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>3500</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="M24" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>113</v>
       </c>
@@ -1864,17 +1939,20 @@
       <c r="I25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="1">
+        <v>83.75</v>
+      </c>
+      <c r="K25" s="2">
         <v>3700</v>
       </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
         <v>3750</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>116</v>
       </c>
@@ -1902,17 +1980,20 @@
       <c r="I26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K26" s="2">
         <v>3528</v>
       </c>
-      <c r="K26" s="2">
+      <c r="L26" s="2">
         <v>3500</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>120</v>
       </c>
@@ -1940,17 +2021,20 @@
       <c r="I27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K27" s="2">
         <v>3528</v>
       </c>
-      <c r="K27" s="2">
+      <c r="L27" s="2">
         <v>3500</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="M27" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>123</v>
       </c>
@@ -1978,17 +2062,20 @@
       <c r="I28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K28" s="2">
         <v>4000</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
         <v>3800</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="M28" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
@@ -2016,17 +2103,20 @@
       <c r="I29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="1">
+        <v>69.75</v>
+      </c>
+      <c r="K29" s="2">
         <v>3450</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
         <v>3500</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -2054,17 +2144,20 @@
       <c r="I30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J30" s="2">
-        <v>3500</v>
+      <c r="J30" s="1">
+        <v>62.5</v>
       </c>
       <c r="K30" s="2">
         <v>3500</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="L30" s="2">
+        <v>3500</v>
+      </c>
+      <c r="M30" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -2092,17 +2185,20 @@
       <c r="I31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="1">
+        <v>78.25</v>
+      </c>
+      <c r="K31" s="2">
         <v>4100</v>
       </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
         <v>4000</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -2130,17 +2226,20 @@
       <c r="I32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="K32" s="2">
         <v>3880</v>
       </c>
-      <c r="K32" s="2">
+      <c r="L32" s="2">
         <v>3700</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="M32" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
@@ -2168,17 +2267,20 @@
       <c r="I33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="1">
+        <v>80.75</v>
+      </c>
+      <c r="K33" s="2">
         <v>4300</v>
       </c>
-      <c r="K33" s="2">
+      <c r="L33" s="2">
         <v>4200</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -2206,17 +2308,20 @@
       <c r="I34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="1">
+        <v>67.5</v>
+      </c>
+      <c r="K34" s="2">
         <v>3450</v>
       </c>
-      <c r="K34" s="2">
+      <c r="L34" s="2">
         <v>3510</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="M34" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>143</v>
       </c>
@@ -2244,17 +2349,20 @@
       <c r="I35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="2">
-        <v>4000</v>
+      <c r="J35" s="1">
+        <v>68.75</v>
       </c>
       <c r="K35" s="2">
         <v>4000</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="L35" s="2">
+        <v>4000</v>
+      </c>
+      <c r="M35" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
@@ -2282,17 +2390,20 @@
       <c r="I36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="1">
+        <v>65</v>
+      </c>
+      <c r="K36" s="2">
         <v>3500</v>
       </c>
-      <c r="K36" s="2">
+      <c r="L36" s="2">
         <v>3600</v>
       </c>
-      <c r="L36" s="3" t="s">
+      <c r="M36" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>75</v>
       </c>
@@ -2320,17 +2431,20 @@
       <c r="I37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="1">
+        <v>66.25</v>
+      </c>
+      <c r="K37" s="2">
         <v>3850</v>
       </c>
-      <c r="K37" s="2">
+      <c r="L37" s="2">
         <v>3600</v>
       </c>
-      <c r="L37" s="3" t="s">
+      <c r="M37" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>152</v>
       </c>
@@ -2358,17 +2472,20 @@
       <c r="I38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="K38" s="2">
         <v>3325</v>
       </c>
-      <c r="K38" s="2">
+      <c r="L38" s="2">
         <v>3300</v>
       </c>
-      <c r="L38" s="3" t="s">
+      <c r="M38" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>155</v>
       </c>
@@ -2396,17 +2513,20 @@
       <c r="I39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="1">
+        <v>73.25</v>
+      </c>
+      <c r="K39" s="2">
         <v>3245</v>
       </c>
-      <c r="K39" s="2">
+      <c r="L39" s="2">
         <v>3400</v>
       </c>
-      <c r="L39" s="3" t="s">
+      <c r="M39" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
@@ -2434,17 +2554,20 @@
       <c r="I40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="1">
+        <v>85</v>
+      </c>
+      <c r="K40" s="2">
         <v>4300</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="M40" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>91</v>
       </c>
@@ -2472,17 +2595,20 @@
       <c r="I41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="1">
+        <v>85</v>
+      </c>
+      <c r="K41" s="2">
         <v>3550</v>
       </c>
-      <c r="K41" s="2">
+      <c r="L41" s="2">
         <v>3500</v>
       </c>
-      <c r="L41" s="3" t="s">
+      <c r="M41" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>163</v>
       </c>
@@ -2510,17 +2636,20 @@
       <c r="I42" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="1">
+        <v>71.25</v>
+      </c>
+      <c r="K42" s="2">
         <v>3656</v>
       </c>
-      <c r="K42" s="2">
+      <c r="L42" s="2">
         <v>3599</v>
       </c>
-      <c r="L42" s="3" t="s">
+      <c r="M42" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>166</v>
       </c>
@@ -2548,17 +2677,20 @@
       <c r="I43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="1">
+        <v>68.75</v>
+      </c>
+      <c r="K43" s="2">
         <v>3700</v>
       </c>
-      <c r="K43" s="2">
+      <c r="L43" s="2">
         <v>3500</v>
       </c>
-      <c r="L43" s="3" t="s">
+      <c r="M43" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -2586,17 +2718,20 @@
       <c r="I44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="1">
+        <v>73.25</v>
+      </c>
+      <c r="K44" s="2">
         <v>4542</v>
       </c>
-      <c r="K44" s="2">
+      <c r="L44" s="2">
         <v>4300</v>
       </c>
-      <c r="L44" s="3" t="s">
+      <c r="M44" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
@@ -2624,62 +2759,65 @@
       <c r="I45" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="1">
+        <v>80</v>
+      </c>
+      <c r="K45" s="2">
         <v>4542</v>
       </c>
-      <c r="K45" s="2">
+      <c r="L45" s="2">
         <v>4300</v>
       </c>
-      <c r="L45" s="3" t="s">
+      <c r="M45" s="3" t="s">
         <v>173</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{E0C593BD-EA27-48A5-888B-11AFE5BE87C3}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{E032A2AE-BF01-48C0-B294-59F667DD569D}"/>
-    <hyperlink ref="L4" r:id="rId3" xr:uid="{7CA6E174-00A0-4B1D-98F9-B64A22BAF022}"/>
-    <hyperlink ref="L5" r:id="rId4" xr:uid="{2F16641C-24F0-433D-BE27-4512EEFC9074}"/>
-    <hyperlink ref="L6" r:id="rId5" xr:uid="{6381023A-6904-4BEF-888B-139695A654A7}"/>
-    <hyperlink ref="L7" r:id="rId6" xr:uid="{3662EE0B-E67E-4580-82CE-753E496A6D2B}"/>
-    <hyperlink ref="L8" r:id="rId7" xr:uid="{8CE7C4EA-22E4-4DCD-AEFC-773BC8F49F8A}"/>
-    <hyperlink ref="L9" r:id="rId8" xr:uid="{71932C26-E00F-4648-A1B9-11A5BF77DB6D}"/>
-    <hyperlink ref="L10" r:id="rId9" xr:uid="{DBDEC4A9-204C-49F5-95B9-E3837251FD22}"/>
-    <hyperlink ref="L11" r:id="rId10" xr:uid="{8DC88931-B4DD-47B8-8980-C12BCEBB3639}"/>
-    <hyperlink ref="L12" r:id="rId11" xr:uid="{27F2E58D-C939-4A54-BC2F-CB2DCFE345C7}"/>
-    <hyperlink ref="L13" r:id="rId12" xr:uid="{58B378AB-15E1-46CF-A383-6B4414B940CA}"/>
-    <hyperlink ref="L14" r:id="rId13" xr:uid="{10E00EE0-C0AC-414B-AB33-B014E3875CEF}"/>
-    <hyperlink ref="L15" r:id="rId14" xr:uid="{CBAF22BE-1143-4AB9-B62E-867D2CF43296}"/>
-    <hyperlink ref="L16" r:id="rId15" xr:uid="{E1BD4EDF-3078-4E84-A497-B19F6CCBCA29}"/>
-    <hyperlink ref="L17" r:id="rId16" xr:uid="{86E21271-9BE4-4F4F-A3B6-0DC52BEF79F1}"/>
-    <hyperlink ref="L18" r:id="rId17" xr:uid="{2DE69177-D300-4981-B2CB-CC17B4E27972}"/>
-    <hyperlink ref="L19" r:id="rId18" xr:uid="{D533928F-8808-4664-A728-2DC7705B4F13}"/>
-    <hyperlink ref="L20" r:id="rId19" xr:uid="{3947E39D-90D6-43A1-B7C9-9659563485A5}"/>
-    <hyperlink ref="L21" r:id="rId20" xr:uid="{1C9174A0-014E-4F42-9549-479A10FE8246}"/>
-    <hyperlink ref="L22" r:id="rId21" xr:uid="{054F09BD-B13E-49E5-A584-9349B37823C1}"/>
-    <hyperlink ref="L23" r:id="rId22" xr:uid="{1D61E4C0-8CE6-4B8F-AD84-45997698AEF0}"/>
-    <hyperlink ref="L24" r:id="rId23" xr:uid="{AC3859DE-177D-4710-9C4B-48DC0BF7853A}"/>
-    <hyperlink ref="L25" r:id="rId24" xr:uid="{A2E599E0-DB40-4DE9-AE9B-8C58D2EB0CE0}"/>
-    <hyperlink ref="L26" r:id="rId25" xr:uid="{D371DB70-E0E4-4F7B-B5BD-D6CF15465C6C}"/>
-    <hyperlink ref="L27" r:id="rId26" xr:uid="{46DC20CB-3C93-4511-AE2B-ADADECD86686}"/>
-    <hyperlink ref="L28" r:id="rId27" xr:uid="{A0429508-2FE8-4F49-B5EF-2B0C336C7439}"/>
-    <hyperlink ref="L29" r:id="rId28" xr:uid="{DF0DA1FD-A6F2-4077-A732-4791440E20EE}"/>
-    <hyperlink ref="L30" r:id="rId29" xr:uid="{70B4EF2E-76E4-479B-8EB6-05A297085009}"/>
-    <hyperlink ref="L31" r:id="rId30" xr:uid="{849AE478-8965-4714-9296-2D906D82626F}"/>
-    <hyperlink ref="L32" r:id="rId31" xr:uid="{DD7C1F05-1E0A-4ED3-A8DB-FF017419D09E}"/>
-    <hyperlink ref="L33" r:id="rId32" xr:uid="{B40861C0-12CC-4193-B97C-2A33CE80F0E7}"/>
-    <hyperlink ref="L34" r:id="rId33" xr:uid="{979B8E99-B9C2-4C87-8047-6F8ED2E25609}"/>
-    <hyperlink ref="L35" r:id="rId34" xr:uid="{B80AE3F5-FEE9-4886-8631-B76864D5C191}"/>
-    <hyperlink ref="L36" r:id="rId35" xr:uid="{025CD302-B84A-4220-822C-AC22A08E6994}"/>
-    <hyperlink ref="L37" r:id="rId36" xr:uid="{8C305BEE-00A3-430E-B7A2-C96ED1F7022A}"/>
-    <hyperlink ref="L38" r:id="rId37" xr:uid="{B38CEC81-168A-4202-96E4-7F4CB7B0ED18}"/>
-    <hyperlink ref="L39" r:id="rId38" xr:uid="{3B68B723-276D-499C-B1D7-B757E64DB208}"/>
-    <hyperlink ref="L40" r:id="rId39" xr:uid="{38FE3792-4B92-42C3-89C2-BD52EC3354A8}"/>
-    <hyperlink ref="L41" r:id="rId40" xr:uid="{5CA03AEA-8C83-434F-AB15-E3D95A4C06BE}"/>
-    <hyperlink ref="L42" r:id="rId41" xr:uid="{4B85C157-02A7-478B-BFE6-CD3DC4F48416}"/>
-    <hyperlink ref="L43" r:id="rId42" xr:uid="{5440A8BD-AEE8-44C3-9C74-A65477BAECEE}"/>
-    <hyperlink ref="L44" r:id="rId43" xr:uid="{ED3DC30C-E05F-47BB-90D4-7F732C44C311}"/>
-    <hyperlink ref="L45" r:id="rId44" xr:uid="{22D5C534-5DFD-41B5-9C96-441941B5EA20}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{E0C593BD-EA27-48A5-888B-11AFE5BE87C3}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{E032A2AE-BF01-48C0-B294-59F667DD569D}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{7CA6E174-00A0-4B1D-98F9-B64A22BAF022}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{2F16641C-24F0-433D-BE27-4512EEFC9074}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{6381023A-6904-4BEF-888B-139695A654A7}"/>
+    <hyperlink ref="M7" r:id="rId6" xr:uid="{3662EE0B-E67E-4580-82CE-753E496A6D2B}"/>
+    <hyperlink ref="M8" r:id="rId7" xr:uid="{8CE7C4EA-22E4-4DCD-AEFC-773BC8F49F8A}"/>
+    <hyperlink ref="M9" r:id="rId8" xr:uid="{71932C26-E00F-4648-A1B9-11A5BF77DB6D}"/>
+    <hyperlink ref="M10" r:id="rId9" xr:uid="{DBDEC4A9-204C-49F5-95B9-E3837251FD22}"/>
+    <hyperlink ref="M11" r:id="rId10" xr:uid="{8DC88931-B4DD-47B8-8980-C12BCEBB3639}"/>
+    <hyperlink ref="M12" r:id="rId11" xr:uid="{27F2E58D-C939-4A54-BC2F-CB2DCFE345C7}"/>
+    <hyperlink ref="M13" r:id="rId12" xr:uid="{58B378AB-15E1-46CF-A383-6B4414B940CA}"/>
+    <hyperlink ref="M14" r:id="rId13" xr:uid="{10E00EE0-C0AC-414B-AB33-B014E3875CEF}"/>
+    <hyperlink ref="M15" r:id="rId14" xr:uid="{CBAF22BE-1143-4AB9-B62E-867D2CF43296}"/>
+    <hyperlink ref="M16" r:id="rId15" xr:uid="{E1BD4EDF-3078-4E84-A497-B19F6CCBCA29}"/>
+    <hyperlink ref="M17" r:id="rId16" xr:uid="{86E21271-9BE4-4F4F-A3B6-0DC52BEF79F1}"/>
+    <hyperlink ref="M18" r:id="rId17" xr:uid="{2DE69177-D300-4981-B2CB-CC17B4E27972}"/>
+    <hyperlink ref="M19" r:id="rId18" xr:uid="{D533928F-8808-4664-A728-2DC7705B4F13}"/>
+    <hyperlink ref="M20" r:id="rId19" xr:uid="{3947E39D-90D6-43A1-B7C9-9659563485A5}"/>
+    <hyperlink ref="M21" r:id="rId20" xr:uid="{1C9174A0-014E-4F42-9549-479A10FE8246}"/>
+    <hyperlink ref="M22" r:id="rId21" xr:uid="{054F09BD-B13E-49E5-A584-9349B37823C1}"/>
+    <hyperlink ref="M23" r:id="rId22" xr:uid="{1D61E4C0-8CE6-4B8F-AD84-45997698AEF0}"/>
+    <hyperlink ref="M24" r:id="rId23" xr:uid="{AC3859DE-177D-4710-9C4B-48DC0BF7853A}"/>
+    <hyperlink ref="M25" r:id="rId24" xr:uid="{A2E599E0-DB40-4DE9-AE9B-8C58D2EB0CE0}"/>
+    <hyperlink ref="M26" r:id="rId25" xr:uid="{D371DB70-E0E4-4F7B-B5BD-D6CF15465C6C}"/>
+    <hyperlink ref="M27" r:id="rId26" xr:uid="{46DC20CB-3C93-4511-AE2B-ADADECD86686}"/>
+    <hyperlink ref="M28" r:id="rId27" xr:uid="{A0429508-2FE8-4F49-B5EF-2B0C336C7439}"/>
+    <hyperlink ref="M29" r:id="rId28" xr:uid="{DF0DA1FD-A6F2-4077-A732-4791440E20EE}"/>
+    <hyperlink ref="M30" r:id="rId29" xr:uid="{70B4EF2E-76E4-479B-8EB6-05A297085009}"/>
+    <hyperlink ref="M31" r:id="rId30" xr:uid="{849AE478-8965-4714-9296-2D906D82626F}"/>
+    <hyperlink ref="M32" r:id="rId31" xr:uid="{DD7C1F05-1E0A-4ED3-A8DB-FF017419D09E}"/>
+    <hyperlink ref="M33" r:id="rId32" xr:uid="{B40861C0-12CC-4193-B97C-2A33CE80F0E7}"/>
+    <hyperlink ref="M34" r:id="rId33" xr:uid="{979B8E99-B9C2-4C87-8047-6F8ED2E25609}"/>
+    <hyperlink ref="M35" r:id="rId34" xr:uid="{B80AE3F5-FEE9-4886-8631-B76864D5C191}"/>
+    <hyperlink ref="M36" r:id="rId35" xr:uid="{025CD302-B84A-4220-822C-AC22A08E6994}"/>
+    <hyperlink ref="M37" r:id="rId36" xr:uid="{8C305BEE-00A3-430E-B7A2-C96ED1F7022A}"/>
+    <hyperlink ref="M38" r:id="rId37" xr:uid="{B38CEC81-168A-4202-96E4-7F4CB7B0ED18}"/>
+    <hyperlink ref="M39" r:id="rId38" xr:uid="{3B68B723-276D-499C-B1D7-B757E64DB208}"/>
+    <hyperlink ref="M40" r:id="rId39" xr:uid="{38FE3792-4B92-42C3-89C2-BD52EC3354A8}"/>
+    <hyperlink ref="M41" r:id="rId40" xr:uid="{5CA03AEA-8C83-434F-AB15-E3D95A4C06BE}"/>
+    <hyperlink ref="M42" r:id="rId41" xr:uid="{4B85C157-02A7-478B-BFE6-CD3DC4F48416}"/>
+    <hyperlink ref="M43" r:id="rId42" xr:uid="{5440A8BD-AEE8-44C3-9C74-A65477BAECEE}"/>
+    <hyperlink ref="M44" r:id="rId43" xr:uid="{ED3DC30C-E05F-47BB-90D4-7F732C44C311}"/>
+    <hyperlink ref="M45" r:id="rId44" xr:uid="{22D5C534-5DFD-41B5-9C96-441941B5EA20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId45"/>

</xml_diff>